<commit_message>
Fixing vehicle transaction DLA ref.
</commit_message>
<xml_diff>
--- a/Output/FedAcqTrends/Fed_Acq_Trends_Contracts.xlsx
+++ b/Output/FedAcqTrends/Fed_Acq_Trends_Contracts.xlsx
@@ -209,13 +209,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="165" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="173" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -251,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -259,7 +260,8 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4322,85 +4324,85 @@
       <c r="O2" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="7" t="n">
+      <c r="P2" s="8" t="n">
         <v>115584932087.843</v>
       </c>
-      <c r="Q2" s="7" t="n">
+      <c r="Q2" s="8" t="n">
         <v>121502367782.02</v>
       </c>
-      <c r="R2" s="7" t="n">
+      <c r="R2" s="8" t="n">
         <v>141593494397.09</v>
       </c>
-      <c r="S2" s="7" t="n">
+      <c r="S2" s="8" t="n">
         <v>161285608480.54</v>
       </c>
-      <c r="T2" s="7" t="n">
+      <c r="T2" s="8" t="n">
         <v>163996030847.09</v>
       </c>
-      <c r="U2" s="7" t="n">
+      <c r="U2" s="8" t="n">
         <v>175328319971.78</v>
       </c>
-      <c r="V2" s="7" t="n">
+      <c r="V2" s="8" t="n">
         <v>192560637208.94</v>
       </c>
-      <c r="W2" s="7" t="n">
+      <c r="W2" s="8" t="n">
         <v>211744401940.64</v>
       </c>
-      <c r="X2" s="7" t="n">
+      <c r="X2" s="8" t="n">
         <v>233778708533.83</v>
       </c>
-      <c r="Y2" s="7" t="n">
+      <c r="Y2" s="8" t="n">
         <v>249159557830.25</v>
       </c>
-      <c r="Z2" s="7" t="n">
+      <c r="Z2" s="8" t="n">
         <v>233830052488.546</v>
       </c>
-      <c r="AA2" s="7" t="n">
+      <c r="AA2" s="8" t="n">
         <v>241482384013.595</v>
       </c>
-      <c r="AB2" s="7" t="n">
+      <c r="AB2" s="8" t="n">
         <v>234644269222.769</v>
       </c>
-      <c r="AC2" s="7" t="n">
+      <c r="AC2" s="8" t="n">
         <v>220649797969.318</v>
       </c>
-      <c r="AD2" s="7" t="n">
+      <c r="AD2" s="8" t="n">
         <v>205868349030.096</v>
       </c>
-      <c r="AE2" s="7" t="n">
+      <c r="AE2" s="8" t="n">
         <v>202950852109.667</v>
       </c>
-      <c r="AF2" s="7" t="n">
+      <c r="AF2" s="8" t="n">
         <v>221377738695.742</v>
       </c>
-      <c r="AG2" s="7" t="n">
+      <c r="AG2" s="8" t="n">
         <v>236813005408.073</v>
       </c>
-      <c r="AH2" s="7" t="n">
+      <c r="AH2" s="8" t="n">
         <v>240263846698.15</v>
       </c>
-      <c r="AI2" s="7" t="n">
+      <c r="AI2" s="8" t="n">
         <v>260617535659.55</v>
       </c>
-      <c r="AJ2" s="7" t="n">
+      <c r="AJ2" s="8" t="n">
         <v>303891362541.91</v>
       </c>
-      <c r="AK2" s="7" t="n">
+      <c r="AK2" s="8" t="n">
         <v>278053239730.06</v>
       </c>
-      <c r="AL2" s="7" t="n">
+      <c r="AL2" s="8" t="n">
         <v>290753329708.25</v>
       </c>
-      <c r="AM2" s="7" t="n">
+      <c r="AM2" s="8" t="n">
         <v>300926082777.59</v>
       </c>
-      <c r="AN2" s="7" t="n">
+      <c r="AN2" s="8" t="n">
         <v>272402781565.84</v>
       </c>
-      <c r="AO2" s="7" t="n">
+      <c r="AO2" s="8" t="n">
         <v>122901870485.08</v>
       </c>
-      <c r="AP2" s="7"/>
+      <c r="AP2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4415,85 +4417,85 @@
       <c r="O3" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="7" t="n">
+      <c r="P3" s="8" t="n">
         <v>12424490879.0119</v>
       </c>
-      <c r="Q3" s="7" t="n">
+      <c r="Q3" s="8" t="n">
         <v>12398785334.88</v>
       </c>
-      <c r="R3" s="7" t="n">
+      <c r="R3" s="8" t="n">
         <v>14572212695.81</v>
       </c>
-      <c r="S3" s="7" t="n">
+      <c r="S3" s="8" t="n">
         <v>17953386972.19</v>
       </c>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="8" t="n">
         <v>10439748453.19</v>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="8" t="n">
         <v>15387923565.0402</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="V3" s="8" t="n">
         <v>16349199022.49</v>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="W3" s="8" t="n">
         <v>17287774018.13</v>
       </c>
-      <c r="X3" s="7" t="n">
+      <c r="X3" s="8" t="n">
         <v>19402260045.67</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="Y3" s="8" t="n">
         <v>18036960407.42</v>
       </c>
-      <c r="Z3" s="7" t="n">
+      <c r="Z3" s="8" t="n">
         <v>18838466035.7132</v>
       </c>
-      <c r="AA3" s="7" t="n">
+      <c r="AA3" s="8" t="n">
         <v>19068572744.5791</v>
       </c>
-      <c r="AB3" s="7" t="n">
+      <c r="AB3" s="8" t="n">
         <v>15609105830.1121</v>
       </c>
-      <c r="AC3" s="7" t="n">
+      <c r="AC3" s="8" t="n">
         <v>14671363072.5204</v>
       </c>
-      <c r="AD3" s="7" t="n">
+      <c r="AD3" s="8" t="n">
         <v>15386698059.2257</v>
       </c>
-      <c r="AE3" s="7" t="n">
+      <c r="AE3" s="8" t="n">
         <v>15371395945.8963</v>
       </c>
-      <c r="AF3" s="7" t="n">
+      <c r="AF3" s="8" t="n">
         <v>15939407819.5676</v>
       </c>
-      <c r="AG3" s="7" t="n">
+      <c r="AG3" s="8" t="n">
         <v>16445854200.7774</v>
       </c>
-      <c r="AH3" s="7" t="n">
+      <c r="AH3" s="8" t="n">
         <v>18122420104.74</v>
       </c>
-      <c r="AI3" s="7" t="n">
+      <c r="AI3" s="8" t="n">
         <v>18307348766.47</v>
       </c>
-      <c r="AJ3" s="7" t="n">
+      <c r="AJ3" s="8" t="n">
         <v>18751614110.04</v>
       </c>
-      <c r="AK3" s="7" t="n">
+      <c r="AK3" s="8" t="n">
         <v>18079383098.6</v>
       </c>
-      <c r="AL3" s="7" t="n">
+      <c r="AL3" s="8" t="n">
         <v>17619524286.9399</v>
       </c>
-      <c r="AM3" s="7" t="n">
+      <c r="AM3" s="8" t="n">
         <v>18564512230.82</v>
       </c>
-      <c r="AN3" s="7" t="n">
+      <c r="AN3" s="8" t="n">
         <v>18885974131.15</v>
       </c>
-      <c r="AO3" s="7" t="n">
+      <c r="AO3" s="8" t="n">
         <v>6877464236.2</v>
       </c>
-      <c r="AP3" s="7"/>
+      <c r="AP3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -4508,85 +4510,85 @@
       <c r="O4" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="7" t="n">
+      <c r="P4" s="8" t="n">
         <v>2924283951.6635</v>
       </c>
-      <c r="Q4" s="7" t="n">
+      <c r="Q4" s="8" t="n">
         <v>3207191850.0918</v>
       </c>
-      <c r="R4" s="7" t="n">
+      <c r="R4" s="8" t="n">
         <v>3874952414.6563</v>
       </c>
-      <c r="S4" s="7" t="n">
+      <c r="S4" s="8" t="n">
         <v>6046089235.4572</v>
       </c>
-      <c r="T4" s="7" t="n">
+      <c r="T4" s="8" t="n">
         <v>6517723173.9598</v>
       </c>
-      <c r="U4" s="7" t="n">
+      <c r="U4" s="8" t="n">
         <v>7361479923.7156</v>
       </c>
-      <c r="V4" s="7" t="n">
+      <c r="V4" s="8" t="n">
         <v>10244737777.7215</v>
       </c>
-      <c r="W4" s="7" t="n">
+      <c r="W4" s="8" t="n">
         <v>9564407533.4996</v>
       </c>
-      <c r="X4" s="7" t="n">
+      <c r="X4" s="8" t="n">
         <v>10960045597.3539</v>
       </c>
-      <c r="Y4" s="7" t="n">
+      <c r="Y4" s="8" t="n">
         <v>11978600453.1904</v>
       </c>
-      <c r="Z4" s="7" t="n">
+      <c r="Z4" s="8" t="n">
         <v>15621451371.1824</v>
       </c>
-      <c r="AA4" s="7" t="n">
+      <c r="AA4" s="8" t="n">
         <v>16861341352.9837</v>
       </c>
-      <c r="AB4" s="7" t="n">
+      <c r="AB4" s="8" t="n">
         <v>18982743607.8388</v>
       </c>
-      <c r="AC4" s="7" t="n">
+      <c r="AC4" s="8" t="n">
         <v>17611974768.2794</v>
       </c>
-      <c r="AD4" s="7" t="n">
+      <c r="AD4" s="8" t="n">
         <v>19114152539.0507</v>
       </c>
-      <c r="AE4" s="7" t="n">
+      <c r="AE4" s="8" t="n">
         <v>21876752873.9362</v>
       </c>
-      <c r="AF4" s="7" t="n">
+      <c r="AF4" s="8" t="n">
         <v>23706172088.7046</v>
       </c>
-      <c r="AG4" s="7" t="n">
+      <c r="AG4" s="8" t="n">
         <v>27628005661.5531</v>
       </c>
-      <c r="AH4" s="7" t="n">
+      <c r="AH4" s="8" t="n">
         <v>31723701465.4611</v>
       </c>
-      <c r="AI4" s="7" t="n">
+      <c r="AI4" s="8" t="n">
         <v>30294003975.1963</v>
       </c>
-      <c r="AJ4" s="7" t="n">
+      <c r="AJ4" s="8" t="n">
         <v>32912233053.9116</v>
       </c>
-      <c r="AK4" s="7" t="n">
+      <c r="AK4" s="8" t="n">
         <v>35673646859.41</v>
       </c>
-      <c r="AL4" s="7" t="n">
+      <c r="AL4" s="8" t="n">
         <v>36438665738.0698</v>
       </c>
-      <c r="AM4" s="7" t="n">
+      <c r="AM4" s="8" t="n">
         <v>41953935024.797</v>
       </c>
-      <c r="AN4" s="7" t="n">
+      <c r="AN4" s="8" t="n">
         <v>44249119911.4933</v>
       </c>
-      <c r="AO4" s="7" t="n">
+      <c r="AO4" s="8" t="n">
         <v>16045018091.44</v>
       </c>
-      <c r="AP4" s="7"/>
+      <c r="AP4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -4601,85 +4603,85 @@
       <c r="O5" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="7" t="n">
+      <c r="P5" s="8" t="n">
         <v>12804541051.7536</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="8" t="n">
         <v>16873262693.0018</v>
       </c>
-      <c r="R5" s="7" t="n">
+      <c r="R5" s="8" t="n">
         <v>22130372261.5838</v>
       </c>
-      <c r="S5" s="7" t="n">
+      <c r="S5" s="8" t="n">
         <v>29036319534.7097</v>
       </c>
-      <c r="T5" s="7" t="n">
+      <c r="T5" s="8" t="n">
         <v>28896257654.6845</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="8" t="n">
         <v>27985121320.1103</v>
       </c>
-      <c r="V5" s="7" t="n">
+      <c r="V5" s="8" t="n">
         <v>28608695358.7399</v>
       </c>
-      <c r="W5" s="7" t="n">
+      <c r="W5" s="8" t="n">
         <v>28419281384.4194</v>
       </c>
-      <c r="X5" s="7" t="n">
+      <c r="X5" s="8" t="n">
         <v>28301482390.3614</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="Y5" s="8" t="n">
         <v>29145223208.8904</v>
       </c>
-      <c r="Z5" s="7" t="n">
+      <c r="Z5" s="8" t="n">
         <v>30481486022.048</v>
       </c>
-      <c r="AA5" s="7" t="n">
+      <c r="AA5" s="8" t="n">
         <v>28787764705.0707</v>
       </c>
-      <c r="AB5" s="7" t="n">
+      <c r="AB5" s="8" t="n">
         <v>27565436312.6723</v>
       </c>
-      <c r="AC5" s="7" t="n">
+      <c r="AC5" s="8" t="n">
         <v>26341597412.0245</v>
       </c>
-      <c r="AD5" s="7" t="n">
+      <c r="AD5" s="8" t="n">
         <v>28514322156.6811</v>
       </c>
-      <c r="AE5" s="7" t="n">
+      <c r="AE5" s="8" t="n">
         <v>27170572289.2424</v>
       </c>
-      <c r="AF5" s="7" t="n">
+      <c r="AF5" s="8" t="n">
         <v>28404542612.8277</v>
       </c>
-      <c r="AG5" s="7" t="n">
+      <c r="AG5" s="8" t="n">
         <v>29276109719.641</v>
       </c>
-      <c r="AH5" s="7" t="n">
+      <c r="AH5" s="8" t="n">
         <v>32092451726.2584</v>
       </c>
-      <c r="AI5" s="7" t="n">
+      <c r="AI5" s="8" t="n">
         <v>35270020674.4173</v>
       </c>
-      <c r="AJ5" s="7" t="n">
+      <c r="AJ5" s="8" t="n">
         <v>39992299401.8298</v>
       </c>
-      <c r="AK5" s="7" t="n">
+      <c r="AK5" s="8" t="n">
         <v>42574994512.184</v>
       </c>
-      <c r="AL5" s="7" t="n">
+      <c r="AL5" s="8" t="n">
         <v>45468863712.7538</v>
       </c>
-      <c r="AM5" s="7" t="n">
+      <c r="AM5" s="8" t="n">
         <v>50127935085.405</v>
       </c>
-      <c r="AN5" s="7" t="n">
+      <c r="AN5" s="8" t="n">
         <v>52657836136.9445</v>
       </c>
-      <c r="AO5" s="7" t="n">
+      <c r="AO5" s="8" t="n">
         <v>18691017774.63</v>
       </c>
-      <c r="AP5" s="7"/>
+      <c r="AP5" s="8"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4694,85 +4696,85 @@
       <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="7" t="n">
+      <c r="P6" s="8" t="n">
         <v>12499350083.2159</v>
       </c>
-      <c r="Q6" s="7" t="n">
+      <c r="Q6" s="8" t="n">
         <v>13610392675.4568</v>
       </c>
-      <c r="R6" s="7" t="n">
+      <c r="R6" s="8" t="n">
         <v>17269119548.3314</v>
       </c>
-      <c r="S6" s="7" t="n">
+      <c r="S6" s="8" t="n">
         <v>22442982846.4399</v>
       </c>
-      <c r="T6" s="7" t="n">
+      <c r="T6" s="8" t="n">
         <v>28374850068.4161</v>
       </c>
-      <c r="U6" s="7" t="n">
+      <c r="U6" s="8" t="n">
         <v>36667866725.8685</v>
       </c>
-      <c r="V6" s="7" t="n">
+      <c r="V6" s="8" t="n">
         <v>43450040207.2155</v>
       </c>
-      <c r="W6" s="7" t="n">
+      <c r="W6" s="8" t="n">
         <v>49537652392.8318</v>
       </c>
-      <c r="X6" s="7" t="n">
+      <c r="X6" s="8" t="n">
         <v>58296941967.6551</v>
       </c>
-      <c r="Y6" s="7" t="n">
+      <c r="Y6" s="8" t="n">
         <v>70755225318.678</v>
       </c>
-      <c r="Z6" s="7" t="n">
+      <c r="Z6" s="8" t="n">
         <v>97069660263.6013</v>
       </c>
-      <c r="AA6" s="7" t="n">
+      <c r="AA6" s="8" t="n">
         <v>80093220983.5518</v>
       </c>
-      <c r="AB6" s="7" t="n">
+      <c r="AB6" s="8" t="n">
         <v>74546629220.6372</v>
       </c>
-      <c r="AC6" s="7" t="n">
+      <c r="AC6" s="8" t="n">
         <v>66847036617.2891</v>
       </c>
-      <c r="AD6" s="7" t="n">
+      <c r="AD6" s="8" t="n">
         <v>64428236170.0944</v>
       </c>
-      <c r="AE6" s="7" t="n">
+      <c r="AE6" s="8" t="n">
         <v>63377140940.6581</v>
       </c>
-      <c r="AF6" s="7" t="n">
+      <c r="AF6" s="8" t="n">
         <v>69942453671.4085</v>
       </c>
-      <c r="AG6" s="7" t="n">
+      <c r="AG6" s="8" t="n">
         <v>72695491339.1477</v>
       </c>
-      <c r="AH6" s="7" t="n">
+      <c r="AH6" s="8" t="n">
         <v>85093046747.5623</v>
       </c>
-      <c r="AI6" s="7" t="n">
+      <c r="AI6" s="8" t="n">
         <v>91689007118.2997</v>
       </c>
-      <c r="AJ6" s="7" t="n">
+      <c r="AJ6" s="8" t="n">
         <v>97258044710.1001</v>
       </c>
-      <c r="AK6" s="7" t="n">
+      <c r="AK6" s="8" t="n">
         <v>92661038675.0052</v>
       </c>
-      <c r="AL6" s="7" t="n">
+      <c r="AL6" s="8" t="n">
         <v>104949993341.112</v>
       </c>
-      <c r="AM6" s="7" t="n">
+      <c r="AM6" s="8" t="n">
         <v>123328551353.892</v>
       </c>
-      <c r="AN6" s="7" t="n">
+      <c r="AN6" s="8" t="n">
         <v>132978957310.474</v>
       </c>
-      <c r="AO6" s="7" t="n">
+      <c r="AO6" s="8" t="n">
         <v>49241265631.31</v>
       </c>
-      <c r="AP6" s="7"/>
+      <c r="AP6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -4787,85 +4789,85 @@
       <c r="O7" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="7" t="n">
+      <c r="P7" s="8" t="n">
         <v>42335529372.3551</v>
       </c>
-      <c r="Q7" s="7" t="n">
+      <c r="Q7" s="8" t="n">
         <v>48917333171.8777</v>
       </c>
-      <c r="R7" s="7" t="n">
+      <c r="R7" s="8" t="n">
         <v>57454020947.247</v>
       </c>
-      <c r="S7" s="7" t="n">
+      <c r="S7" s="8" t="n">
         <v>77397735316.5918</v>
       </c>
-      <c r="T7" s="7" t="n">
+      <c r="T7" s="8" t="n">
         <v>96729076010.967</v>
       </c>
-      <c r="U7" s="7" t="n">
+      <c r="U7" s="8" t="n">
         <v>126006897249.582</v>
       </c>
-      <c r="V7" s="7" t="n">
+      <c r="V7" s="8" t="n">
         <v>138189605286.346</v>
       </c>
-      <c r="W7" s="7" t="n">
+      <c r="W7" s="8" t="n">
         <v>152278596019.012</v>
       </c>
-      <c r="X7" s="7" t="n">
+      <c r="X7" s="8" t="n">
         <v>176992562159.486</v>
       </c>
-      <c r="Y7" s="7" t="n">
+      <c r="Y7" s="8" t="n">
         <v>175807040178.201</v>
       </c>
-      <c r="Z7" s="7" t="n">
+      <c r="Z7" s="8" t="n">
         <v>165348458600.938</v>
       </c>
-      <c r="AA7" s="7" t="n">
+      <c r="AA7" s="8" t="n">
         <v>153864370550.964</v>
       </c>
-      <c r="AB7" s="7" t="n">
+      <c r="AB7" s="8" t="n">
         <v>149755532268.463</v>
       </c>
-      <c r="AC7" s="7" t="n">
+      <c r="AC7" s="8" t="n">
         <v>117832148608.451</v>
       </c>
-      <c r="AD7" s="7" t="n">
+      <c r="AD7" s="8" t="n">
         <v>113132246206.875</v>
       </c>
-      <c r="AE7" s="7" t="n">
+      <c r="AE7" s="8" t="n">
         <v>109430096987.006</v>
       </c>
-      <c r="AF7" s="7" t="n">
+      <c r="AF7" s="8" t="n">
         <v>116420314684.446</v>
       </c>
-      <c r="AG7" s="7" t="n">
+      <c r="AG7" s="8" t="n">
         <v>128243356113.859</v>
       </c>
-      <c r="AH7" s="7" t="n">
+      <c r="AH7" s="8" t="n">
         <v>149051590332.517</v>
       </c>
-      <c r="AI7" s="7" t="n">
+      <c r="AI7" s="8" t="n">
         <v>153875006598.917</v>
       </c>
-      <c r="AJ7" s="7" t="n">
+      <c r="AJ7" s="8" t="n">
         <v>178955739455.671</v>
       </c>
-      <c r="AK7" s="7" t="n">
+      <c r="AK7" s="8" t="n">
         <v>178756105576.716</v>
       </c>
-      <c r="AL7" s="7" t="n">
+      <c r="AL7" s="8" t="n">
         <v>199544845267.319</v>
       </c>
-      <c r="AM7" s="7" t="n">
+      <c r="AM7" s="8" t="n">
         <v>226196676468.225</v>
       </c>
-      <c r="AN7" s="7" t="n">
+      <c r="AN7" s="8" t="n">
         <v>234676048634.219</v>
       </c>
-      <c r="AO7" s="7" t="n">
+      <c r="AO7" s="8" t="n">
         <v>101273651433.94</v>
       </c>
-      <c r="AP7" s="7"/>
+      <c r="AP7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -4880,85 +4882,85 @@
       <c r="O8" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="7" t="n">
+      <c r="P8" s="8" t="n">
         <v>7030877168.3082</v>
       </c>
-      <c r="Q8" s="7" t="n">
+      <c r="Q8" s="8" t="n">
         <v>6612007723.823</v>
       </c>
-      <c r="R8" s="7" t="n">
+      <c r="R8" s="8" t="n">
         <v>7284000092.3487</v>
       </c>
-      <c r="S8" s="7" t="n">
+      <c r="S8" s="8" t="n">
         <v>5366434247.8165</v>
       </c>
-      <c r="T8" s="7" t="n">
+      <c r="T8" s="8" t="n">
         <v>4415654379.2757</v>
       </c>
-      <c r="U8" s="7" t="n">
+      <c r="U8" s="8" t="n">
         <v>2683711410.774</v>
       </c>
-      <c r="V8" s="7" t="n">
+      <c r="V8" s="8" t="n">
         <v>1747131444.4168</v>
       </c>
-      <c r="W8" s="7" t="n">
+      <c r="W8" s="8" t="n">
         <v>1000337098.5642</v>
       </c>
-      <c r="X8" s="7" t="n">
+      <c r="X8" s="8" t="n">
         <v>592811723.8758</v>
       </c>
-      <c r="Y8" s="7" t="n">
+      <c r="Y8" s="8" t="n">
         <v>337021017.1379</v>
       </c>
-      <c r="Z8" s="7" t="n">
+      <c r="Z8" s="8" t="n">
         <v>271869696.8448</v>
       </c>
-      <c r="AA8" s="7" t="n">
+      <c r="AA8" s="8" t="n">
         <v>123556347.7826</v>
       </c>
-      <c r="AB8" s="7" t="n">
+      <c r="AB8" s="8" t="n">
         <v>99091517.7124</v>
       </c>
-      <c r="AC8" s="7" t="n">
+      <c r="AC8" s="8" t="n">
         <v>47651396.2464</v>
       </c>
-      <c r="AD8" s="7" t="n">
+      <c r="AD8" s="8" t="n">
         <v>55333426.4992</v>
       </c>
-      <c r="AE8" s="7" t="n">
+      <c r="AE8" s="8" t="n">
         <v>61667152.8337</v>
       </c>
-      <c r="AF8" s="7" t="n">
+      <c r="AF8" s="8" t="n">
         <v>29264169.4202</v>
       </c>
-      <c r="AG8" s="7" t="n">
+      <c r="AG8" s="8" t="n">
         <v>7714685.453</v>
       </c>
-      <c r="AH8" s="7" t="n">
+      <c r="AH8" s="8" t="n">
         <v>3121458.2472</v>
       </c>
-      <c r="AI8" s="7" t="n">
+      <c r="AI8" s="8" t="n">
         <v>1801758.2113</v>
       </c>
-      <c r="AJ8" s="7" t="n">
+      <c r="AJ8" s="8" t="n">
         <v>1589203.1028</v>
       </c>
-      <c r="AK8" s="7" t="n">
+      <c r="AK8" s="8" t="n">
         <v>-4965343.4824</v>
       </c>
-      <c r="AL8" s="7" t="n">
+      <c r="AL8" s="8" t="n">
         <v>-17602406.375</v>
       </c>
-      <c r="AM8" s="7" t="n">
+      <c r="AM8" s="8" t="n">
         <v>-15651681.9895</v>
       </c>
-      <c r="AN8" s="7" t="n">
+      <c r="AN8" s="8" t="n">
         <v>-1314944.4</v>
       </c>
-      <c r="AO8" s="7" t="n">
+      <c r="AO8" s="8" t="n">
         <v>-14742791.4</v>
       </c>
-      <c r="AP8" s="7"/>
+      <c r="AP8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -4969,85 +4971,85 @@
       </c>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9" s="7" t="n">
+      <c r="P9" s="8" t="n">
         <v>18006362</v>
       </c>
-      <c r="Q9" s="7" t="n">
+      <c r="Q9" s="8" t="n">
         <v>773740.3125</v>
       </c>
-      <c r="R9" s="7" t="n">
+      <c r="R9" s="8" t="n">
         <v>1369209.8414</v>
       </c>
-      <c r="S9" s="7" t="n">
+      <c r="S9" s="8" t="n">
         <v>6076922.5</v>
       </c>
-      <c r="T9" s="7" t="n">
+      <c r="T9" s="8" t="n">
         <v>5022298.0339</v>
       </c>
-      <c r="U9" s="7" t="n">
+      <c r="U9" s="8" t="n">
         <v>402007.8403</v>
       </c>
-      <c r="V9" s="7" t="n">
+      <c r="V9" s="8" t="n">
         <v>647421.89</v>
       </c>
-      <c r="W9" s="7" t="n">
+      <c r="W9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="X9" s="7" t="n">
+      <c r="X9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Y9" s="7" t="n">
+      <c r="Y9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Z9" s="7" t="n">
+      <c r="Z9" s="8" t="n">
         <v>236000</v>
       </c>
-      <c r="AA9" s="7" t="n">
+      <c r="AA9" s="8" t="n">
         <v>248000</v>
       </c>
-      <c r="AB9" s="7" t="n">
+      <c r="AB9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AC9" s="7" t="n">
+      <c r="AC9" s="8" t="n">
         <v>717723</v>
       </c>
-      <c r="AD9" s="7" t="n">
+      <c r="AD9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AE9" s="7" t="n">
+      <c r="AE9" s="8" t="n">
         <v>2364.39</v>
       </c>
-      <c r="AF9" s="7" t="n">
+      <c r="AF9" s="8" t="n">
         <v>-5000</v>
       </c>
-      <c r="AG9" s="7" t="n">
+      <c r="AG9" s="8" t="n">
         <v>1810263.7657</v>
       </c>
-      <c r="AH9" s="7" t="n">
+      <c r="AH9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AI9" s="7" t="n">
+      <c r="AI9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AJ9" s="7" t="n">
+      <c r="AJ9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AK9" s="7" t="n">
+      <c r="AK9" s="8" t="n">
         <v>30674.99</v>
       </c>
-      <c r="AL9" s="7" t="n">
+      <c r="AL9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AM9" s="7" t="n">
+      <c r="AM9" s="8" t="n">
         <v>-10000</v>
       </c>
-      <c r="AN9" s="7" t="n">
+      <c r="AN9" s="8" t="n">
         <v>3572327.86</v>
       </c>
-      <c r="AO9" s="7" t="n">
+      <c r="AO9" s="8" t="n">
         <v>-6130361.98</v>
       </c>
-      <c r="AP9" s="7"/>
+      <c r="AP9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -5062,85 +5064,85 @@
       <c r="O10" t="s">
         <v>60</v>
       </c>
-      <c r="P10" s="7" t="str">
+      <c r="P10" s="8" t="str">
         <f>Sum(P2:P9)</f>
       </c>
-      <c r="Q10" s="7" t="str">
+      <c r="Q10" s="8" t="str">
         <f>Sum(Q2:Q9)</f>
       </c>
-      <c r="R10" s="7" t="str">
+      <c r="R10" s="8" t="str">
         <f>Sum(R2:R9)</f>
       </c>
-      <c r="S10" s="7" t="str">
+      <c r="S10" s="8" t="str">
         <f>Sum(S2:S9)</f>
       </c>
-      <c r="T10" s="7" t="str">
+      <c r="T10" s="8" t="str">
         <f>Sum(T2:T9)</f>
       </c>
-      <c r="U10" s="7" t="str">
+      <c r="U10" s="8" t="str">
         <f>Sum(U2:U9)</f>
       </c>
-      <c r="V10" s="7" t="str">
+      <c r="V10" s="8" t="str">
         <f>Sum(V2:V9)</f>
       </c>
-      <c r="W10" s="7" t="str">
+      <c r="W10" s="8" t="str">
         <f>Sum(W2:W9)</f>
       </c>
-      <c r="X10" s="7" t="str">
+      <c r="X10" s="8" t="str">
         <f>Sum(X2:X9)</f>
       </c>
-      <c r="Y10" s="7" t="str">
+      <c r="Y10" s="8" t="str">
         <f>Sum(Y2:Y9)</f>
       </c>
-      <c r="Z10" s="7" t="str">
+      <c r="Z10" s="8" t="str">
         <f>Sum(Z2:Z9)</f>
       </c>
-      <c r="AA10" s="7" t="str">
+      <c r="AA10" s="8" t="str">
         <f>Sum(AA2:AA9)</f>
       </c>
-      <c r="AB10" s="7" t="str">
+      <c r="AB10" s="8" t="str">
         <f>Sum(AB2:AB9)</f>
       </c>
-      <c r="AC10" s="7" t="str">
+      <c r="AC10" s="8" t="str">
         <f>Sum(AC2:AC9)</f>
       </c>
-      <c r="AD10" s="7" t="str">
+      <c r="AD10" s="8" t="str">
         <f>Sum(AD2:AD9)</f>
       </c>
-      <c r="AE10" s="7" t="str">
+      <c r="AE10" s="8" t="str">
         <f>Sum(AE2:AE9)</f>
       </c>
-      <c r="AF10" s="7" t="str">
+      <c r="AF10" s="8" t="str">
         <f>Sum(AF2:AF9)</f>
       </c>
-      <c r="AG10" s="7" t="str">
+      <c r="AG10" s="8" t="str">
         <f>Sum(AG2:AG9)</f>
       </c>
-      <c r="AH10" s="7" t="str">
+      <c r="AH10" s="8" t="str">
         <f>Sum(AH2:AH9)</f>
       </c>
-      <c r="AI10" s="7" t="str">
+      <c r="AI10" s="8" t="str">
         <f>Sum(AI2:AI9)</f>
       </c>
-      <c r="AJ10" s="7" t="str">
+      <c r="AJ10" s="8" t="str">
         <f>Sum(AJ2:AJ9)</f>
       </c>
-      <c r="AK10" s="7" t="str">
+      <c r="AK10" s="8" t="str">
         <f>Sum(AK2:AK9)</f>
       </c>
-      <c r="AL10" s="7" t="str">
+      <c r="AL10" s="8" t="str">
         <f>Sum(AL2:AL9)</f>
       </c>
-      <c r="AM10" s="7" t="str">
+      <c r="AM10" s="8" t="str">
         <f>Sum(AM2:AM9)</f>
       </c>
-      <c r="AN10" s="7" t="str">
+      <c r="AN10" s="8" t="str">
         <f>Sum(AN2:AN9)</f>
       </c>
-      <c r="AO10" s="7" t="str">
+      <c r="AO10" s="8" t="str">
         <f>Sum(AO2:AO9)</f>
       </c>
-      <c r="AP10" s="7"/>
+      <c r="AP10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>